<commit_message>
Testing for iteration 10
</commit_message>
<xml_diff>
--- a/Metrics/Bug Log & Metric.xlsx
+++ b/Metrics/Bug Log & Metric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\FYP\venv\Beyond-Ideas\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2776EF0E-D017-4D56-8A11-DD3B14554FD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1297928F-F8DF-42B1-829A-F401CEFC33E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="438" windowWidth="28800" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="438" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metric" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
   <si>
     <t>No.</t>
   </si>
@@ -252,6 +251,27 @@
   </si>
   <si>
     <t>Only able to upload from specific folder</t>
+  </si>
+  <si>
+    <t>View Dataset</t>
+  </si>
+  <si>
+    <t>Viewing of weather and movement data not available</t>
+  </si>
+  <si>
+    <t>30mins</t>
+  </si>
+  <si>
+    <t>Unable to combine datasets for some of the data source</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Inventory data's variable not shown in dependant or independent variables when selected as datasource</t>
+  </si>
+  <si>
+    <t>Unable to deselect a datasource/variable</t>
   </si>
 </sst>
 </file>
@@ -568,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -705,6 +725,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,7 +864,7 @@
               <c:f>'Bug Metric'!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -870,22 +893,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2060,7 +2068,7 @@
     <col min="4" max="4" width="28.27734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.27734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="7" max="7" width="39.21875" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="56.5546875" customWidth="1"/>
   </cols>
@@ -2235,7 +2243,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:26" ht="30.9" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="52">
         <v>3</v>
       </c>
@@ -2283,7 +2291,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:26" ht="29.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="52">
         <v>4</v>
       </c>
@@ -2326,7 +2334,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:26" ht="33.299999999999997" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="52">
         <v>5</v>
       </c>
@@ -2371,7 +2379,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="52">
         <v>6</v>
       </c>
@@ -2414,7 +2422,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="52">
         <v>7</v>
       </c>
@@ -2456,7 +2464,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="52">
         <v>8</v>
       </c>
@@ -2503,7 +2511,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:26" ht="23.4" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="52">
         <v>9</v>
       </c>
@@ -2550,19 +2558,29 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="52">
         <v>10</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
+      <c r="B12" s="54">
+        <v>4</v>
+      </c>
+      <c r="C12" s="54">
+        <v>1</v>
+      </c>
+      <c r="D12" s="54">
+        <v>3</v>
+      </c>
+      <c r="E12" s="54">
+        <v>0</v>
+      </c>
       <c r="F12" s="54">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
-      <c r="G12" s="55"/>
+      <c r="G12" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="7" t="s">
         <v>32</v>
@@ -2587,7 +2605,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:26" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="52">
         <v>11</v>
       </c>
@@ -2624,7 +2642,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="52">
         <v>12</v>
       </c>
@@ -2657,7 +2675,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="52">
         <v>13</v>
       </c>
@@ -2690,7 +2708,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="52">
         <v>14</v>
       </c>
@@ -2723,7 +2741,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="52">
         <v>15</v>
       </c>
@@ -2761,19 +2779,19 @@
         <v>28</v>
       </c>
       <c r="B18" s="54">
-        <f>SUM(B3:B11)</f>
-        <v>15</v>
+        <f>SUM(B3:B12)</f>
+        <v>19</v>
       </c>
       <c r="C18" s="54">
-        <f>SUM(C3:C11)</f>
-        <v>4</v>
+        <f>SUM(C3:C12)</f>
+        <v>5</v>
       </c>
       <c r="D18" s="54">
-        <f>SUM(D3:D11)</f>
-        <v>3</v>
+        <f>SUM(D3:D12)</f>
+        <v>6</v>
       </c>
       <c r="E18" s="54">
-        <f>SUM(E3:E11)</f>
+        <f>SUM(E3:E12)</f>
         <v>8</v>
       </c>
       <c r="F18" s="54">
@@ -30339,11 +30357,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="5" ySplit="10" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane xSplit="5" ySplit="10" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -30703,8 +30721,12 @@
       <c r="H9" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="26"/>
+      <c r="I9" s="24">
+        <v>43449</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="K9" s="22" t="s">
         <v>43</v>
       </c>
@@ -30712,7 +30734,9 @@
         <v>10</v>
       </c>
       <c r="M9" s="26"/>
-      <c r="N9" s="23"/>
+      <c r="N9" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O9" s="26"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -30749,7 +30773,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="26"/>
-      <c r="N10" s="29" t="s">
+      <c r="N10" s="22" t="s">
         <v>51</v>
       </c>
       <c r="O10" s="26"/>
@@ -30775,8 +30799,12 @@
       <c r="H11" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="24">
+        <v>43449</v>
+      </c>
+      <c r="J11" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="K11" s="64" t="s">
         <v>43</v>
       </c>
@@ -30784,7 +30812,9 @@
         <v>10</v>
       </c>
       <c r="M11" s="26"/>
-      <c r="N11" s="23"/>
+      <c r="N11" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -30821,7 +30851,7 @@
         <v>10</v>
       </c>
       <c r="M12" s="23"/>
-      <c r="N12" s="29" t="s">
+      <c r="N12" s="22" t="s">
         <v>51</v>
       </c>
       <c r="O12" s="29"/>
@@ -30847,8 +30877,12 @@
       <c r="H13" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="29"/>
+      <c r="I13" s="24">
+        <v>43462</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="K13" s="29" t="s">
         <v>43</v>
       </c>
@@ -30856,7 +30890,9 @@
         <v>10</v>
       </c>
       <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
+      <c r="N13" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O13" s="29"/>
     </row>
     <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -30882,7 +30918,8 @@
       <c r="H14" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="29"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
       <c r="K14" s="64" t="s">
         <v>38</v>
       </c>
@@ -30890,7 +30927,9 @@
         <v>5</v>
       </c>
       <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
+      <c r="N14" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O14" s="29"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -30914,8 +30953,12 @@
       <c r="H15" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="29"/>
+      <c r="I15" s="24">
+        <v>43478</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>46</v>
+      </c>
       <c r="K15" s="64" t="s">
         <v>43</v>
       </c>
@@ -30923,7 +30966,9 @@
         <v>10</v>
       </c>
       <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
+      <c r="N15" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O15" s="29"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -30947,8 +30992,8 @@
       <c r="H16" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="71"/>
       <c r="K16" s="64" t="s">
         <v>55</v>
       </c>
@@ -30956,24 +31001,40 @@
         <v>1</v>
       </c>
       <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
+      <c r="N16" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="O16" s="29"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="42">
         <v>16</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="23">
+        <v>10</v>
+      </c>
       <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="29"/>
+      <c r="G17" s="24">
+        <v>43492</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="I17" s="24"/>
       <c r="J17" s="29"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
+      <c r="K17" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="23">
+        <v>5</v>
+      </c>
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
       <c r="O17" s="29"/>
@@ -30982,17 +31043,31 @@
       <c r="A18" s="42">
         <v>17</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="29">
+        <v>10</v>
+      </c>
       <c r="C18" s="23"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
+      <c r="D18" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="F18" s="30"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="29"/>
+      <c r="G18" s="24">
+        <v>43492</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="I18" s="24"/>
       <c r="J18" s="29"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="32"/>
+      <c r="K18" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="32">
+        <v>5</v>
+      </c>
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="29"/>
@@ -31001,17 +31076,31 @@
       <c r="A19" s="42">
         <v>18</v>
       </c>
-      <c r="B19" s="34"/>
+      <c r="B19" s="34">
+        <v>10</v>
+      </c>
       <c r="C19" s="37"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+      <c r="D19" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>74</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="34"/>
+      <c r="G19" s="24">
+        <v>43492</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="I19" s="38"/>
       <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="37"/>
+      <c r="K19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="32">
+        <v>5</v>
+      </c>
       <c r="M19" s="37"/>
       <c r="N19" s="34"/>
       <c r="O19" s="34"/>
@@ -31020,17 +31109,31 @@
       <c r="A20" s="42">
         <v>19</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="29">
+        <v>10</v>
+      </c>
       <c r="C20" s="23"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="D20" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>75</v>
+      </c>
       <c r="F20" s="29"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="29"/>
+      <c r="G20" s="24">
+        <v>43492</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="I20" s="24"/>
       <c r="J20" s="29"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="32"/>
+      <c r="K20" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="L20" s="32">
+        <v>1</v>
+      </c>
       <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="29"/>

</xml_diff>

<commit_message>
Updated Testing Added insertion into database function
</commit_message>
<xml_diff>
--- a/Metrics/Bug Log & Metric.xlsx
+++ b/Metrics/Bug Log & Metric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\FYP\venv\Beyond-Ideas\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D068B379-3050-4F49-9234-765C6696A516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C65FBB6-B292-46E1-8F38-C48419CC89E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="28800" windowHeight="16518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
   <si>
     <t>No.</t>
   </si>
@@ -272,6 +272,27 @@
   </si>
   <si>
     <t>Unable to deselect a datasource/variable</t>
+  </si>
+  <si>
+    <t>Table View</t>
+  </si>
+  <si>
+    <t>Unable to save the same table into the database twice</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Web Crawling(Weather)</t>
+  </si>
+  <si>
+    <t>Button misaligned</t>
+  </si>
+  <si>
+    <t>Options to save to database or as a csv file not working.</t>
+  </si>
+  <si>
+    <t>Did not crawl for some of the years with february 29</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1067,7 @@
               <c:f>'Bug Metric'!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1079,6 +1100,18 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2242,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2837,17 +2870,25 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="52">
         <v>12</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
+      <c r="B14" s="53">
+        <v>3</v>
+      </c>
+      <c r="C14" s="53">
+        <v>2</v>
+      </c>
+      <c r="D14" s="53">
+        <v>1</v>
+      </c>
+      <c r="E14" s="53">
+        <v>1</v>
+      </c>
       <c r="F14" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G14" s="54"/>
       <c r="H14" s="1"/>
@@ -2870,7 +2911,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="52">
         <v>13</v>
       </c>
@@ -2903,7 +2944,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="52">
         <v>14</v>
       </c>
@@ -2936,7 +2977,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="52">
         <v>15</v>
       </c>
@@ -2974,24 +3015,24 @@
         <v>28</v>
       </c>
       <c r="B18" s="53">
-        <f>SUM(B3:B13)</f>
-        <v>20</v>
+        <f>SUM(B3:B14)</f>
+        <v>23</v>
       </c>
       <c r="C18" s="53">
-        <f>SUM(C3:C13)</f>
-        <v>6</v>
+        <f>SUM(C3:C14)</f>
+        <v>8</v>
       </c>
       <c r="D18" s="53">
-        <f>SUM(D3:D13)</f>
-        <v>6</v>
+        <f>SUM(D3:D14)</f>
+        <v>7</v>
       </c>
       <c r="E18" s="53">
-        <f>SUM(E3:E13)</f>
-        <v>8</v>
+        <f>SUM(E3:E14)</f>
+        <v>9</v>
       </c>
       <c r="F18" s="53">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="G18" s="53"/>
       <c r="H18" s="1"/>
@@ -30552,11 +30593,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P994"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="5" ySplit="10" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+      <pane xSplit="5" ySplit="10" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -31341,38 +31382,66 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="42">
-        <v>20</v>
-      </c>
-      <c r="B21" s="29"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="29">
+        <v>11</v>
+      </c>
       <c r="C21" s="23"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="D21" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>75</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="29"/>
+      <c r="G21" s="24">
+        <v>43505</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="I21" s="24"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="23"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" s="32">
+        <v>1</v>
+      </c>
       <c r="M21" s="23"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="29"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="42">
         <v>21</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="29">
+        <v>12</v>
+      </c>
       <c r="C22" s="23"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="D22" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>77</v>
+      </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="29"/>
+      <c r="G22" s="38">
+        <v>43520</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="I22" s="24"/>
       <c r="J22" s="29"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="23"/>
+      <c r="K22" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22" s="23">
+        <v>5</v>
+      </c>
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
       <c r="O22" s="29"/>
@@ -31381,55 +31450,97 @@
       <c r="A23" s="42">
         <v>22</v>
       </c>
-      <c r="B23" s="34"/>
+      <c r="B23" s="34">
+        <v>12</v>
+      </c>
       <c r="C23" s="37"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
+      <c r="D23" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="34"/>
+      <c r="G23" s="38">
+        <v>43520</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="I23" s="38"/>
       <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="37"/>
+      <c r="K23" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" s="37">
+        <v>1</v>
+      </c>
       <c r="M23" s="37"/>
       <c r="N23" s="34"/>
       <c r="O23" s="34"/>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="42">
         <v>23</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="34">
+        <v>12</v>
+      </c>
       <c r="C24" s="23"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
+      <c r="D24" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
+      <c r="G24" s="38">
+        <v>43520</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="38"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="37">
+        <v>10</v>
+      </c>
       <c r="M24" s="23"/>
       <c r="N24" s="36"/>
       <c r="O24" s="36"/>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="42">
-        <v>24</v>
-      </c>
-      <c r="B25" s="34"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="34">
+        <v>12</v>
+      </c>
       <c r="C25" s="23"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>82</v>
+      </c>
       <c r="F25" s="34"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
+      <c r="G25" s="38">
+        <v>43520</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="38"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="37">
+        <v>1</v>
+      </c>
       <c r="M25" s="23"/>
       <c r="N25" s="36"/>
       <c r="O25" s="36"/>

</xml_diff>

<commit_message>
Regression testing & Debugging for iteration 14.
</commit_message>
<xml_diff>
--- a/Metrics/Bug Log & Metric.xlsx
+++ b/Metrics/Bug Log & Metric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\FYP\venv\Beyond-Ideas\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3ABA19-45F0-444F-A48F-1FD7D6B29FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916D8F1-BDD8-4566-B97F-35E21B63C5EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="28800" windowHeight="16518" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>No.</t>
   </si>
@@ -302,6 +302,21 @@
   </si>
   <si>
     <t>If user typed special characters as filename to be saved in the database, the system crashes</t>
+  </si>
+  <si>
+    <t>Data retrieval</t>
+  </si>
+  <si>
+    <t>Unable to put space as file name</t>
+  </si>
+  <si>
+    <t>Using same dataset for correlation will have an error</t>
+  </si>
+  <si>
+    <t>View dataset</t>
+  </si>
+  <si>
+    <t>If user select to view 100 row, the vertical scroll bar will not work, have to use the mouse's scroll.</t>
   </si>
 </sst>
 </file>
@@ -624,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -771,6 +786,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,7 +1089,7 @@
               <c:f>'Bug Metric'!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1112,6 +1128,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2275,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2956,17 +2975,25 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="51">
         <v>14</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
+      <c r="B16" s="52">
+        <v>3</v>
+      </c>
+      <c r="C16" s="52">
+        <v>2</v>
+      </c>
+      <c r="D16" s="52">
+        <v>1</v>
+      </c>
+      <c r="E16" s="52">
+        <v>0</v>
+      </c>
       <c r="F16" s="52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G16" s="53"/>
       <c r="H16" s="1"/>
@@ -3027,24 +3054,24 @@
         <v>28</v>
       </c>
       <c r="B18" s="52">
-        <f>SUM(B3:B15)</f>
-        <v>26</v>
+        <f>SUM(B3:B16)</f>
+        <v>29</v>
       </c>
       <c r="C18" s="52">
-        <f>SUM(C3:C15)</f>
-        <v>10</v>
+        <f>SUM(C3:C16)</f>
+        <v>12</v>
       </c>
       <c r="D18" s="52">
-        <f>SUM(D3:D15)</f>
-        <v>7</v>
+        <f>SUM(D3:D16)</f>
+        <v>8</v>
       </c>
       <c r="E18" s="52">
-        <f>SUM(E3:E15)</f>
+        <f>SUM(E3:E16)</f>
         <v>10</v>
       </c>
       <c r="F18" s="52">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="G18" s="52"/>
       <c r="H18" s="1"/>
@@ -30606,10 +30633,8 @@
   <dimension ref="A1:P994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane xSplit="5" ySplit="10" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -30619,10 +30644,11 @@
     <col min="3" max="3" width="4.1640625" style="11" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="84.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="74.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.83203125" style="11" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.5" style="11"/>
+    <col min="9" max="10" width="0" style="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="11"/>
     <col min="12" max="12" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.83203125" style="11" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
@@ -31564,7 +31590,9 @@
         <v>1</v>
       </c>
       <c r="M25" s="23"/>
-      <c r="N25" s="35"/>
+      <c r="N25" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O25" s="35"/>
     </row>
     <row r="26" spans="1:15" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -31597,7 +31625,9 @@
         <v>1</v>
       </c>
       <c r="M26" s="36"/>
-      <c r="N26" s="38"/>
+      <c r="N26" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O26" s="38"/>
     </row>
     <row r="27" spans="1:15" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -31630,7 +31660,9 @@
         <v>10</v>
       </c>
       <c r="M27" s="36"/>
-      <c r="N27" s="38"/>
+      <c r="N27" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O27" s="34"/>
     </row>
     <row r="28" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
@@ -31663,61 +31695,108 @@
         <v>1</v>
       </c>
       <c r="M28" s="23"/>
-      <c r="N28" s="35"/>
+      <c r="N28" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O28" s="35"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41">
         <v>28</v>
       </c>
-      <c r="B29" s="34"/>
+      <c r="B29" s="34">
+        <v>14</v>
+      </c>
       <c r="C29" s="23"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="D29" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>88</v>
+      </c>
       <c r="F29" s="34"/>
-      <c r="H29" s="34"/>
+      <c r="G29" s="76">
+        <v>43539</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="I29" s="24"/>
       <c r="J29" s="35"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="23"/>
+      <c r="K29" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="23">
+        <v>5</v>
+      </c>
       <c r="M29" s="23"/>
-      <c r="N29" s="35"/>
+      <c r="N29" s="23"/>
       <c r="O29" s="35"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="41">
         <v>29</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="34">
+        <v>14</v>
+      </c>
       <c r="C30" s="23"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
+      <c r="D30" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F30" s="34"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="34"/>
+      <c r="G30" s="24">
+        <v>43548</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="I30" s="24"/>
       <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="23"/>
+      <c r="K30" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" s="23">
+        <v>1</v>
+      </c>
       <c r="M30" s="23"/>
-      <c r="N30" s="35"/>
+      <c r="N30" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O30" s="29"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="41">
         <v>30</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="34">
+        <v>14</v>
+      </c>
       <c r="C31" s="23"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
+      <c r="D31" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>90</v>
+      </c>
       <c r="F31" s="34"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="34"/>
+      <c r="G31" s="24">
+        <v>43548</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="I31" s="24"/>
       <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="23"/>
+      <c r="K31" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" s="23">
+        <v>1</v>
+      </c>
       <c r="M31" s="23"/>
       <c r="N31" s="35"/>
       <c r="O31" s="29"/>

</xml_diff>

<commit_message>
Regression testing for iteration 15
</commit_message>
<xml_diff>
--- a/Metrics/Bug Log & Metric.xlsx
+++ b/Metrics/Bug Log & Metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\FYP\venv\Beyond-Ideas\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916D8F1-BDD8-4566-B97F-35E21B63C5EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFB64C1-60F0-4408-9F66-975028FCBDBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="28800" windowHeight="16518" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="28800" windowHeight="16518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug Metric" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
   <si>
     <t>No.</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>If user select to view 100 row, the vertical scroll bar will not work, have to use the mouse's scroll.</t>
+  </si>
+  <si>
+    <t>Use the planned debugging time</t>
   </si>
 </sst>
 </file>
@@ -777,6 +780,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -786,7 +790,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,7 +1092,7 @@
               <c:f>'Bug Metric'!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1131,6 +1134,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2294,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2305,19 +2311,19 @@
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" customWidth="1"/>
+    <col min="7" max="7" width="46" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="10" max="10" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="73"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="75"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -2384,7 +2390,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:26" ht="18.3" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -2432,7 +2438,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="51">
         <v>2</v>
       </c>
@@ -2480,7 +2486,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:26" ht="19.8" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="51">
         <v>3</v>
       </c>
@@ -2528,7 +2534,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:26" ht="23.7" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="51">
         <v>4</v>
       </c>
@@ -2571,7 +2577,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="46" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="51">
         <v>5</v>
       </c>
@@ -2616,7 +2622,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="23.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="51">
         <v>6</v>
       </c>
@@ -2659,7 +2665,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="21.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="51">
         <v>7</v>
       </c>
@@ -2701,7 +2707,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="51">
         <v>8</v>
       </c>
@@ -2748,7 +2754,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="51">
         <v>9</v>
       </c>
@@ -2795,7 +2801,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="51">
         <v>10</v>
       </c>
@@ -2842,7 +2848,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="43" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="51">
         <v>11</v>
       </c>
@@ -2889,7 +2895,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="51">
         <v>12</v>
       </c>
@@ -2932,7 +2938,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="51">
         <v>13</v>
       </c>
@@ -2995,7 +3001,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="53" t="s">
+        <v>91</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -3016,19 +3024,29 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" ht="18.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="51">
         <v>15</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
+      <c r="B17" s="52">
+        <v>0</v>
+      </c>
+      <c r="C17" s="52">
+        <v>0</v>
+      </c>
+      <c r="D17" s="52">
+        <v>0</v>
+      </c>
+      <c r="E17" s="52">
+        <v>0</v>
+      </c>
       <c r="F17" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="53"/>
+      <c r="G17" s="53" t="s">
+        <v>31</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3049,24 +3067,24 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:26" ht="21.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="51" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="52">
-        <f>SUM(B3:B16)</f>
+        <f>SUM(B3:B17)</f>
         <v>29</v>
       </c>
       <c r="C18" s="52">
-        <f>SUM(C3:C16)</f>
+        <f>SUM(C3:C17)</f>
         <v>12</v>
       </c>
       <c r="D18" s="52">
-        <f>SUM(D3:D16)</f>
+        <f>SUM(D3:D17)</f>
         <v>8</v>
       </c>
       <c r="E18" s="52">
-        <f>SUM(E3:E16)</f>
+        <f>SUM(E3:E17)</f>
         <v>10</v>
       </c>
       <c r="F18" s="52">
@@ -30632,9 +30650,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -31715,7 +31733,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="34"/>
-      <c r="G29" s="76">
+      <c r="G29" s="73">
         <v>43539</v>
       </c>
       <c r="H29" s="34" t="s">
@@ -31730,7 +31748,9 @@
         <v>5</v>
       </c>
       <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
+      <c r="N29" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O29" s="35"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -31798,7 +31818,9 @@
         <v>1</v>
       </c>
       <c r="M31" s="23"/>
-      <c r="N31" s="35"/>
+      <c r="N31" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="O31" s="29"/>
     </row>
     <row r="32" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">

</xml_diff>